<commit_message>
end of day dump, working on finding articles for pathways
</commit_message>
<xml_diff>
--- a/phenopedia cataract related genes/Phenopedia_ClusterONE.xlsx
+++ b/phenopedia cataract related genes/Phenopedia_ClusterONE.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="320" uniqueCount="209">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="329" uniqueCount="216">
   <si>
     <t># nodes</t>
   </si>
@@ -624,9 +624,6 @@
     <t>transepithelial L-ascorbic acid transport</t>
   </si>
   <si>
-    <t>&gt;0.05</t>
-  </si>
-  <si>
     <t>high-density lipoprotein particle clearance</t>
   </si>
   <si>
@@ -646,6 +643,30 @@
   </si>
   <si>
     <t>galactose catabolic process via UDP-galactose</t>
+  </si>
+  <si>
+    <t>&gt;0.1</t>
+  </si>
+  <si>
+    <t>10.1091/mbc.e09-12-1031</t>
+  </si>
+  <si>
+    <t>10.1073/pnas.82.21.7193</t>
+  </si>
+  <si>
+    <t>(none)</t>
+  </si>
+  <si>
+    <t>10.1016/j.semcdb.2006.10.011</t>
+  </si>
+  <si>
+    <t>10.1080/02713680500477347</t>
+  </si>
+  <si>
+    <t>10.1042/BJ20040347</t>
+  </si>
+  <si>
+    <t>10.1016/0039-6257(88)90095-1</t>
   </si>
 </sst>
 </file>
@@ -1453,10 +1474,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AD46"/>
+  <dimension ref="A1:AE46"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="D45" sqref="D45"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E49" sqref="E49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1464,7 +1485,7 @@
     <col min="3" max="3" width="44.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1477,11 +1498,11 @@
       <c r="D1" t="s">
         <v>198</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>26</v>
       </c>
@@ -1494,86 +1515,89 @@
       <c r="D2" s="1">
         <v>8.7899999999999992E-3</v>
       </c>
-      <c r="E2" t="s">
+      <c r="E2" s="1" t="s">
+        <v>209</v>
+      </c>
+      <c r="F2" t="s">
         <v>2</v>
       </c>
-      <c r="F2" t="s">
+      <c r="G2" t="s">
         <v>3</v>
       </c>
-      <c r="G2" t="s">
+      <c r="H2" t="s">
         <v>4</v>
       </c>
-      <c r="H2" t="s">
+      <c r="I2" t="s">
         <v>5</v>
       </c>
-      <c r="I2" t="s">
+      <c r="J2" t="s">
         <v>6</v>
       </c>
-      <c r="J2" t="s">
+      <c r="K2" t="s">
         <v>7</v>
       </c>
-      <c r="K2" t="s">
+      <c r="L2" t="s">
         <v>8</v>
       </c>
-      <c r="L2" t="s">
+      <c r="M2" t="s">
         <v>9</v>
       </c>
-      <c r="M2" t="s">
+      <c r="N2" t="s">
         <v>10</v>
       </c>
-      <c r="N2" t="s">
+      <c r="O2" t="s">
         <v>11</v>
       </c>
-      <c r="O2" t="s">
+      <c r="P2" t="s">
         <v>12</v>
       </c>
-      <c r="P2" t="s">
+      <c r="Q2" t="s">
         <v>13</v>
       </c>
-      <c r="Q2" t="s">
+      <c r="R2" t="s">
         <v>14</v>
       </c>
-      <c r="R2" t="s">
+      <c r="S2" t="s">
         <v>15</v>
       </c>
-      <c r="S2" t="s">
+      <c r="T2" t="s">
         <v>16</v>
       </c>
-      <c r="T2" t="s">
+      <c r="U2" t="s">
         <v>17</v>
       </c>
-      <c r="U2" t="s">
+      <c r="V2" t="s">
         <v>18</v>
       </c>
-      <c r="V2" t="s">
+      <c r="W2" t="s">
         <v>19</v>
       </c>
-      <c r="W2" t="s">
+      <c r="X2" t="s">
         <v>20</v>
       </c>
-      <c r="X2" t="s">
+      <c r="Y2" t="s">
         <v>21</v>
       </c>
-      <c r="Y2" t="s">
+      <c r="Z2" t="s">
         <v>22</v>
       </c>
-      <c r="Z2" t="s">
+      <c r="AA2" t="s">
         <v>23</v>
       </c>
-      <c r="AA2" t="s">
+      <c r="AB2" t="s">
         <v>24</v>
       </c>
-      <c r="AB2" t="s">
+      <c r="AC2" t="s">
         <v>25</v>
       </c>
-      <c r="AC2" t="s">
+      <c r="AD2" t="s">
         <v>26</v>
       </c>
-      <c r="AD2" t="s">
+      <c r="AE2" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="3" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>10</v>
       </c>
@@ -1586,38 +1610,41 @@
       <c r="D3" s="1">
         <v>5.9100000000000003E-3</v>
       </c>
-      <c r="E3" t="s">
+      <c r="E3" s="1" t="s">
+        <v>210</v>
+      </c>
+      <c r="F3" t="s">
         <v>28</v>
       </c>
-      <c r="F3" t="s">
+      <c r="G3" t="s">
         <v>29</v>
       </c>
-      <c r="G3" t="s">
+      <c r="H3" t="s">
         <v>30</v>
       </c>
-      <c r="H3" t="s">
+      <c r="I3" t="s">
         <v>31</v>
       </c>
-      <c r="I3" t="s">
+      <c r="J3" t="s">
         <v>32</v>
       </c>
-      <c r="J3" t="s">
+      <c r="K3" t="s">
         <v>33</v>
       </c>
-      <c r="K3" t="s">
+      <c r="L3" t="s">
         <v>34</v>
       </c>
-      <c r="L3" t="s">
+      <c r="M3" t="s">
         <v>35</v>
       </c>
-      <c r="M3" t="s">
+      <c r="N3" t="s">
         <v>36</v>
       </c>
-      <c r="N3" t="s">
+      <c r="O3" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="4" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>9</v>
       </c>
@@ -1625,37 +1652,37 @@
         <v>2.0633444000000001E-2</v>
       </c>
       <c r="D4" t="s">
-        <v>201</v>
-      </c>
-      <c r="E4" t="s">
+        <v>208</v>
+      </c>
+      <c r="F4" t="s">
         <v>7</v>
       </c>
-      <c r="F4" t="s">
+      <c r="G4" t="s">
         <v>23</v>
       </c>
-      <c r="G4" t="s">
+      <c r="H4" t="s">
         <v>38</v>
       </c>
-      <c r="H4" t="s">
+      <c r="I4" t="s">
         <v>39</v>
       </c>
-      <c r="I4" t="s">
+      <c r="J4" t="s">
         <v>40</v>
       </c>
-      <c r="J4" t="s">
+      <c r="K4" t="s">
         <v>41</v>
       </c>
-      <c r="K4" t="s">
+      <c r="L4" t="s">
         <v>42</v>
       </c>
-      <c r="L4" t="s">
+      <c r="M4" t="s">
         <v>43</v>
       </c>
-      <c r="M4" t="s">
+      <c r="N4" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="5" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>10</v>
       </c>
@@ -1663,40 +1690,40 @@
         <v>0.104251623</v>
       </c>
       <c r="D5" t="s">
-        <v>201</v>
-      </c>
-      <c r="E5" t="s">
+        <v>208</v>
+      </c>
+      <c r="F5" t="s">
         <v>7</v>
       </c>
-      <c r="F5" t="s">
+      <c r="G5" t="s">
         <v>23</v>
       </c>
-      <c r="G5" t="s">
+      <c r="H5" t="s">
         <v>45</v>
       </c>
-      <c r="H5" t="s">
+      <c r="I5" t="s">
         <v>46</v>
       </c>
-      <c r="I5" t="s">
+      <c r="J5" t="s">
         <v>39</v>
       </c>
-      <c r="J5" t="s">
+      <c r="K5" t="s">
         <v>40</v>
       </c>
-      <c r="K5" t="s">
+      <c r="L5" t="s">
         <v>41</v>
       </c>
-      <c r="L5" t="s">
+      <c r="M5" t="s">
         <v>42</v>
       </c>
-      <c r="M5" t="s">
+      <c r="N5" t="s">
         <v>43</v>
       </c>
-      <c r="N5" t="s">
+      <c r="O5" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="6" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>6</v>
       </c>
@@ -1704,28 +1731,28 @@
         <v>0.17965866899999999</v>
       </c>
       <c r="D6" t="s">
-        <v>201</v>
-      </c>
-      <c r="E6" t="s">
+        <v>208</v>
+      </c>
+      <c r="F6" t="s">
         <v>47</v>
       </c>
-      <c r="F6" t="s">
+      <c r="G6" t="s">
         <v>48</v>
       </c>
-      <c r="G6" t="s">
+      <c r="H6" t="s">
         <v>49</v>
       </c>
-      <c r="H6" t="s">
+      <c r="I6" t="s">
         <v>50</v>
       </c>
-      <c r="I6" t="s">
+      <c r="J6" t="s">
         <v>51</v>
       </c>
-      <c r="J6" t="s">
+      <c r="K6" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="7" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
       </c>
@@ -1733,28 +1760,28 @@
         <v>0.18279883199999999</v>
       </c>
       <c r="D7" t="s">
-        <v>201</v>
-      </c>
-      <c r="E7" t="s">
+        <v>208</v>
+      </c>
+      <c r="F7" t="s">
         <v>53</v>
       </c>
-      <c r="F7" t="s">
+      <c r="G7" t="s">
         <v>54</v>
       </c>
-      <c r="G7" t="s">
+      <c r="H7" t="s">
         <v>55</v>
       </c>
-      <c r="H7" t="s">
+      <c r="I7" t="s">
         <v>56</v>
       </c>
-      <c r="I7" t="s">
+      <c r="J7" t="s">
         <v>57</v>
       </c>
-      <c r="J7" t="s">
+      <c r="K7" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="8" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>6</v>
       </c>
@@ -1762,28 +1789,28 @@
         <v>0.18279883199999999</v>
       </c>
       <c r="D8" t="s">
-        <v>201</v>
-      </c>
-      <c r="E8" t="s">
+        <v>208</v>
+      </c>
+      <c r="F8" t="s">
         <v>59</v>
       </c>
-      <c r="F8" t="s">
+      <c r="G8" t="s">
         <v>54</v>
       </c>
-      <c r="G8" t="s">
+      <c r="H8" t="s">
         <v>55</v>
       </c>
-      <c r="H8" t="s">
+      <c r="I8" t="s">
         <v>56</v>
       </c>
-      <c r="I8" t="s">
+      <c r="J8" t="s">
         <v>57</v>
       </c>
-      <c r="J8" t="s">
+      <c r="K8" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="9" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>6</v>
       </c>
@@ -1791,28 +1818,28 @@
         <v>0.18279883199999999</v>
       </c>
       <c r="D9" t="s">
-        <v>201</v>
-      </c>
-      <c r="E9" t="s">
+        <v>208</v>
+      </c>
+      <c r="F9" t="s">
         <v>54</v>
       </c>
-      <c r="F9" t="s">
+      <c r="G9" t="s">
         <v>60</v>
       </c>
-      <c r="G9" t="s">
+      <c r="H9" t="s">
         <v>55</v>
       </c>
-      <c r="H9" t="s">
+      <c r="I9" t="s">
         <v>56</v>
       </c>
-      <c r="I9" t="s">
+      <c r="J9" t="s">
         <v>57</v>
       </c>
-      <c r="J9" t="s">
+      <c r="K9" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="10" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>6</v>
       </c>
@@ -1820,28 +1847,28 @@
         <v>0.18279883199999999</v>
       </c>
       <c r="D10" t="s">
-        <v>201</v>
-      </c>
-      <c r="E10" t="s">
+        <v>208</v>
+      </c>
+      <c r="F10" t="s">
         <v>54</v>
       </c>
-      <c r="F10" t="s">
+      <c r="G10" t="s">
         <v>61</v>
       </c>
-      <c r="G10" t="s">
+      <c r="H10" t="s">
         <v>55</v>
       </c>
-      <c r="H10" t="s">
+      <c r="I10" t="s">
         <v>56</v>
       </c>
-      <c r="I10" t="s">
+      <c r="J10" t="s">
         <v>57</v>
       </c>
-      <c r="J10" t="s">
+      <c r="K10" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="11" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>6</v>
       </c>
@@ -1849,28 +1876,28 @@
         <v>0.18279883199999999</v>
       </c>
       <c r="D11" t="s">
-        <v>201</v>
-      </c>
-      <c r="E11" t="s">
+        <v>208</v>
+      </c>
+      <c r="F11" t="s">
         <v>54</v>
       </c>
-      <c r="F11" t="s">
+      <c r="G11" t="s">
         <v>62</v>
       </c>
-      <c r="G11" t="s">
+      <c r="H11" t="s">
         <v>55</v>
       </c>
-      <c r="H11" t="s">
+      <c r="I11" t="s">
         <v>56</v>
       </c>
-      <c r="I11" t="s">
+      <c r="J11" t="s">
         <v>57</v>
       </c>
-      <c r="J11" t="s">
+      <c r="K11" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="12" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>6</v>
       </c>
@@ -1878,28 +1905,28 @@
         <v>0.18279883199999999</v>
       </c>
       <c r="D12" t="s">
-        <v>201</v>
-      </c>
-      <c r="E12" t="s">
+        <v>208</v>
+      </c>
+      <c r="F12" t="s">
         <v>54</v>
       </c>
-      <c r="F12" t="s">
+      <c r="G12" t="s">
         <v>63</v>
       </c>
-      <c r="G12" t="s">
+      <c r="H12" t="s">
         <v>55</v>
       </c>
-      <c r="H12" t="s">
+      <c r="I12" t="s">
         <v>56</v>
       </c>
-      <c r="I12" t="s">
+      <c r="J12" t="s">
         <v>57</v>
       </c>
-      <c r="J12" t="s">
+      <c r="K12" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="13" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>6</v>
       </c>
@@ -1907,28 +1934,28 @@
         <v>0.18279883199999999</v>
       </c>
       <c r="D13" t="s">
-        <v>201</v>
-      </c>
-      <c r="E13" t="s">
+        <v>208</v>
+      </c>
+      <c r="F13" t="s">
         <v>54</v>
       </c>
-      <c r="F13" t="s">
+      <c r="G13" t="s">
         <v>64</v>
       </c>
-      <c r="G13" t="s">
+      <c r="H13" t="s">
         <v>55</v>
       </c>
-      <c r="H13" t="s">
+      <c r="I13" t="s">
         <v>56</v>
       </c>
-      <c r="I13" t="s">
+      <c r="J13" t="s">
         <v>57</v>
       </c>
-      <c r="J13" t="s">
+      <c r="K13" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="14" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>6</v>
       </c>
@@ -1936,28 +1963,28 @@
         <v>0.18279883199999999</v>
       </c>
       <c r="D14" t="s">
-        <v>201</v>
-      </c>
-      <c r="E14" t="s">
+        <v>208</v>
+      </c>
+      <c r="F14" t="s">
         <v>54</v>
       </c>
-      <c r="F14" t="s">
+      <c r="G14" t="s">
         <v>65</v>
       </c>
-      <c r="G14" t="s">
+      <c r="H14" t="s">
         <v>55</v>
       </c>
-      <c r="H14" t="s">
+      <c r="I14" t="s">
         <v>56</v>
       </c>
-      <c r="I14" t="s">
+      <c r="J14" t="s">
         <v>57</v>
       </c>
-      <c r="J14" t="s">
+      <c r="K14" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="15" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>5</v>
       </c>
@@ -1965,25 +1992,25 @@
         <v>0.333215017</v>
       </c>
       <c r="D15" t="s">
-        <v>201</v>
-      </c>
-      <c r="E15" t="s">
+        <v>208</v>
+      </c>
+      <c r="F15" t="s">
         <v>66</v>
       </c>
-      <c r="F15" t="s">
+      <c r="G15" t="s">
         <v>67</v>
       </c>
-      <c r="G15" t="s">
+      <c r="H15" t="s">
         <v>68</v>
       </c>
-      <c r="H15" t="s">
+      <c r="I15" t="s">
         <v>69</v>
       </c>
-      <c r="I15" t="s">
+      <c r="J15" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="16" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>5</v>
       </c>
@@ -1991,28 +2018,31 @@
         <v>0.333215017</v>
       </c>
       <c r="C16" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="D16" s="1">
         <v>2.7900000000000001E-2</v>
       </c>
-      <c r="E16" t="s">
+      <c r="E16" s="1" t="s">
+        <v>211</v>
+      </c>
+      <c r="F16" t="s">
         <v>71</v>
       </c>
-      <c r="F16" t="s">
+      <c r="G16" t="s">
         <v>72</v>
       </c>
-      <c r="G16" t="s">
+      <c r="H16" t="s">
         <v>73</v>
       </c>
-      <c r="H16" t="s">
+      <c r="I16" t="s">
         <v>74</v>
       </c>
-      <c r="I16" t="s">
+      <c r="J16" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>5</v>
       </c>
@@ -2020,25 +2050,25 @@
         <v>0.333215017</v>
       </c>
       <c r="D17" t="s">
-        <v>201</v>
-      </c>
-      <c r="E17" t="s">
+        <v>208</v>
+      </c>
+      <c r="F17" t="s">
         <v>76</v>
       </c>
-      <c r="F17" t="s">
+      <c r="G17" t="s">
         <v>77</v>
       </c>
-      <c r="G17" t="s">
+      <c r="H17" t="s">
         <v>78</v>
       </c>
-      <c r="H17" t="s">
+      <c r="I17" t="s">
         <v>79</v>
       </c>
-      <c r="I17" t="s">
+      <c r="J17" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>5</v>
       </c>
@@ -2046,25 +2076,25 @@
         <v>0.333215017</v>
       </c>
       <c r="D18" t="s">
-        <v>201</v>
-      </c>
-      <c r="E18" t="s">
+        <v>208</v>
+      </c>
+      <c r="F18" t="s">
         <v>81</v>
       </c>
-      <c r="F18" t="s">
+      <c r="G18" t="s">
         <v>82</v>
       </c>
-      <c r="G18" t="s">
+      <c r="H18" t="s">
         <v>83</v>
       </c>
-      <c r="H18" t="s">
+      <c r="I18" t="s">
         <v>84</v>
       </c>
-      <c r="I18" t="s">
+      <c r="J18" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>5</v>
       </c>
@@ -2072,25 +2102,25 @@
         <v>0.333215017</v>
       </c>
       <c r="D19" t="s">
-        <v>201</v>
-      </c>
-      <c r="E19" t="s">
+        <v>208</v>
+      </c>
+      <c r="F19" t="s">
         <v>86</v>
       </c>
-      <c r="F19" t="s">
+      <c r="G19" t="s">
         <v>87</v>
       </c>
-      <c r="G19" t="s">
+      <c r="H19" t="s">
         <v>88</v>
       </c>
-      <c r="H19" t="s">
+      <c r="I19" t="s">
         <v>89</v>
       </c>
-      <c r="I19" t="s">
+      <c r="J19" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>5</v>
       </c>
@@ -2098,25 +2128,25 @@
         <v>0.33471120900000001</v>
       </c>
       <c r="D20" t="s">
-        <v>201</v>
-      </c>
-      <c r="E20" t="s">
+        <v>208</v>
+      </c>
+      <c r="F20" t="s">
         <v>91</v>
       </c>
-      <c r="F20" t="s">
+      <c r="G20" t="s">
         <v>92</v>
       </c>
-      <c r="G20" t="s">
+      <c r="H20" t="s">
         <v>93</v>
       </c>
-      <c r="H20" t="s">
+      <c r="I20" t="s">
         <v>94</v>
       </c>
-      <c r="I20" t="s">
+      <c r="J20" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>5</v>
       </c>
@@ -2124,25 +2154,25 @@
         <v>0.33471120900000001</v>
       </c>
       <c r="D21" t="s">
-        <v>201</v>
-      </c>
-      <c r="E21" t="s">
+        <v>208</v>
+      </c>
+      <c r="F21" t="s">
         <v>96</v>
       </c>
-      <c r="F21" t="s">
+      <c r="G21" t="s">
         <v>97</v>
       </c>
-      <c r="G21" t="s">
+      <c r="H21" t="s">
         <v>98</v>
       </c>
-      <c r="H21" t="s">
+      <c r="I21" t="s">
         <v>99</v>
       </c>
-      <c r="I21" t="s">
+      <c r="J21" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>7</v>
       </c>
@@ -2150,31 +2180,31 @@
         <v>0.349313602</v>
       </c>
       <c r="D22" t="s">
-        <v>201</v>
-      </c>
-      <c r="E22" t="s">
+        <v>208</v>
+      </c>
+      <c r="F22" t="s">
         <v>100</v>
       </c>
-      <c r="F22" t="s">
+      <c r="G22" t="s">
         <v>101</v>
       </c>
-      <c r="G22" t="s">
+      <c r="H22" t="s">
         <v>102</v>
       </c>
-      <c r="H22" t="s">
+      <c r="I22" t="s">
         <v>103</v>
       </c>
-      <c r="I22" t="s">
+      <c r="J22" t="s">
         <v>104</v>
       </c>
-      <c r="J22" t="s">
+      <c r="K22" t="s">
         <v>105</v>
       </c>
-      <c r="K22" t="s">
+      <c r="L22" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>4</v>
       </c>
@@ -2182,22 +2212,22 @@
         <v>0.5</v>
       </c>
       <c r="D23" t="s">
-        <v>201</v>
-      </c>
-      <c r="E23" t="s">
+        <v>208</v>
+      </c>
+      <c r="F23" t="s">
         <v>76</v>
       </c>
-      <c r="F23" t="s">
+      <c r="G23" t="s">
         <v>107</v>
       </c>
-      <c r="G23" t="s">
+      <c r="H23" t="s">
         <v>108</v>
       </c>
-      <c r="H23" t="s">
+      <c r="I23" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>6</v>
       </c>
@@ -2205,28 +2235,28 @@
         <v>0.53224616300000005</v>
       </c>
       <c r="D24" t="s">
-        <v>201</v>
-      </c>
-      <c r="E24" t="s">
+        <v>208</v>
+      </c>
+      <c r="F24" t="s">
         <v>110</v>
       </c>
-      <c r="F24" t="s">
+      <c r="G24" t="s">
         <v>111</v>
       </c>
-      <c r="G24" t="s">
+      <c r="H24" t="s">
         <v>112</v>
       </c>
-      <c r="H24" t="s">
+      <c r="I24" t="s">
         <v>113</v>
       </c>
-      <c r="I24" t="s">
+      <c r="J24" t="s">
         <v>114</v>
       </c>
-      <c r="J24" t="s">
+      <c r="K24" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>6</v>
       </c>
@@ -2234,31 +2264,34 @@
         <v>0.53230377399999995</v>
       </c>
       <c r="C25" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="D25" s="1">
         <v>1.0800000000000001E-2</v>
       </c>
-      <c r="E25" t="s">
+      <c r="E25" s="1" t="s">
+        <v>211</v>
+      </c>
+      <c r="F25" t="s">
         <v>116</v>
       </c>
-      <c r="F25" t="s">
+      <c r="G25" t="s">
         <v>117</v>
       </c>
-      <c r="G25" t="s">
+      <c r="H25" t="s">
         <v>118</v>
       </c>
-      <c r="H25" t="s">
+      <c r="I25" t="s">
         <v>119</v>
       </c>
-      <c r="I25" t="s">
+      <c r="J25" t="s">
         <v>120</v>
       </c>
-      <c r="J25" t="s">
+      <c r="K25" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>6</v>
       </c>
@@ -2266,28 +2299,28 @@
         <v>0.53241992800000004</v>
       </c>
       <c r="D26" t="s">
-        <v>201</v>
-      </c>
-      <c r="E26" t="s">
+        <v>208</v>
+      </c>
+      <c r="F26" t="s">
         <v>122</v>
       </c>
-      <c r="F26" t="s">
+      <c r="G26" t="s">
         <v>123</v>
       </c>
-      <c r="G26" t="s">
+      <c r="H26" t="s">
         <v>124</v>
       </c>
-      <c r="H26" t="s">
+      <c r="I26" t="s">
         <v>125</v>
       </c>
-      <c r="I26" t="s">
+      <c r="J26" t="s">
         <v>126</v>
       </c>
-      <c r="J26" t="s">
+      <c r="K26" t="s">
         <v>127</v>
       </c>
     </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>6</v>
       </c>
@@ -2295,28 +2328,28 @@
         <v>0.53241992800000004</v>
       </c>
       <c r="D27" t="s">
-        <v>201</v>
-      </c>
-      <c r="E27" t="s">
+        <v>208</v>
+      </c>
+      <c r="F27" t="s">
         <v>90</v>
       </c>
-      <c r="F27" t="s">
+      <c r="G27" t="s">
         <v>128</v>
       </c>
-      <c r="G27" t="s">
+      <c r="H27" t="s">
         <v>129</v>
       </c>
-      <c r="H27" t="s">
+      <c r="I27" t="s">
         <v>130</v>
       </c>
-      <c r="I27" t="s">
+      <c r="J27" t="s">
         <v>131</v>
       </c>
-      <c r="J27" t="s">
+      <c r="K27" t="s">
         <v>132</v>
       </c>
     </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>6</v>
       </c>
@@ -2324,28 +2357,28 @@
         <v>0.53241992800000004</v>
       </c>
       <c r="D28" t="s">
-        <v>201</v>
-      </c>
-      <c r="E28" t="s">
+        <v>208</v>
+      </c>
+      <c r="F28" t="s">
         <v>80</v>
       </c>
-      <c r="F28" t="s">
+      <c r="G28" t="s">
         <v>133</v>
       </c>
-      <c r="G28" t="s">
+      <c r="H28" t="s">
         <v>134</v>
       </c>
-      <c r="H28" t="s">
+      <c r="I28" t="s">
         <v>135</v>
       </c>
-      <c r="I28" t="s">
+      <c r="J28" t="s">
         <v>136</v>
       </c>
-      <c r="J28" t="s">
+      <c r="K28" t="s">
         <v>137</v>
       </c>
     </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>6</v>
       </c>
@@ -2353,31 +2386,34 @@
         <v>0.53241992800000004</v>
       </c>
       <c r="C29" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="D29" s="1">
         <v>2.6200000000000001E-2</v>
       </c>
-      <c r="E29" t="s">
+      <c r="E29" s="1" t="s">
+        <v>212</v>
+      </c>
+      <c r="F29" t="s">
         <v>47</v>
       </c>
-      <c r="F29" t="s">
+      <c r="G29" t="s">
         <v>138</v>
       </c>
-      <c r="G29" t="s">
+      <c r="H29" t="s">
         <v>48</v>
       </c>
-      <c r="H29" t="s">
+      <c r="I29" t="s">
         <v>49</v>
       </c>
-      <c r="I29" t="s">
+      <c r="J29" t="s">
         <v>51</v>
       </c>
-      <c r="J29" t="s">
+      <c r="K29" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>6</v>
       </c>
@@ -2385,28 +2421,28 @@
         <v>0.53241992800000004</v>
       </c>
       <c r="D30" t="s">
-        <v>201</v>
-      </c>
-      <c r="E30" t="s">
+        <v>208</v>
+      </c>
+      <c r="F30" t="s">
         <v>47</v>
       </c>
-      <c r="F30" t="s">
+      <c r="G30" t="s">
         <v>139</v>
       </c>
-      <c r="G30" t="s">
+      <c r="H30" t="s">
         <v>48</v>
       </c>
-      <c r="H30" t="s">
+      <c r="I30" t="s">
         <v>49</v>
       </c>
-      <c r="I30" t="s">
+      <c r="J30" t="s">
         <v>51</v>
       </c>
-      <c r="J30" t="s">
+      <c r="K30" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>6</v>
       </c>
@@ -2414,28 +2450,28 @@
         <v>0.53314418299999999</v>
       </c>
       <c r="D31" t="s">
-        <v>201</v>
-      </c>
-      <c r="E31" t="s">
+        <v>208</v>
+      </c>
+      <c r="F31" t="s">
         <v>140</v>
       </c>
-      <c r="F31" t="s">
+      <c r="G31" t="s">
         <v>141</v>
       </c>
-      <c r="G31" t="s">
+      <c r="H31" t="s">
         <v>142</v>
       </c>
-      <c r="H31" t="s">
+      <c r="I31" t="s">
         <v>96</v>
       </c>
-      <c r="I31" t="s">
+      <c r="J31" t="s">
         <v>143</v>
       </c>
-      <c r="J31" t="s">
+      <c r="K31" t="s">
         <v>144</v>
       </c>
     </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>6</v>
       </c>
@@ -2443,28 +2479,28 @@
         <v>0.53460842399999997</v>
       </c>
       <c r="D32" t="s">
-        <v>201</v>
-      </c>
-      <c r="E32" t="s">
+        <v>208</v>
+      </c>
+      <c r="F32" t="s">
         <v>47</v>
       </c>
-      <c r="F32" t="s">
+      <c r="G32" t="s">
         <v>48</v>
       </c>
-      <c r="G32" t="s">
+      <c r="H32" t="s">
         <v>145</v>
       </c>
-      <c r="H32" t="s">
+      <c r="I32" t="s">
         <v>49</v>
       </c>
-      <c r="I32" t="s">
+      <c r="J32" t="s">
         <v>51</v>
       </c>
-      <c r="J32" t="s">
+      <c r="K32" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>6</v>
       </c>
@@ -2472,28 +2508,28 @@
         <v>0.53460842399999997</v>
       </c>
       <c r="D33" t="s">
-        <v>201</v>
-      </c>
-      <c r="E33" t="s">
+        <v>208</v>
+      </c>
+      <c r="F33" t="s">
         <v>47</v>
       </c>
-      <c r="F33" t="s">
+      <c r="G33" t="s">
         <v>48</v>
       </c>
-      <c r="G33" t="s">
+      <c r="H33" t="s">
         <v>49</v>
       </c>
-      <c r="H33" t="s">
+      <c r="I33" t="s">
         <v>146</v>
       </c>
-      <c r="I33" t="s">
+      <c r="J33" t="s">
         <v>51</v>
       </c>
-      <c r="J33" t="s">
+      <c r="K33" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>4</v>
       </c>
@@ -2501,25 +2537,28 @@
         <v>0.56152267899999997</v>
       </c>
       <c r="C34" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="D34" s="1">
         <v>1.9400000000000001E-2</v>
       </c>
-      <c r="E34" t="s">
+      <c r="E34" s="1" t="s">
+        <v>211</v>
+      </c>
+      <c r="F34" t="s">
         <v>147</v>
       </c>
-      <c r="F34" t="s">
+      <c r="G34" t="s">
         <v>148</v>
       </c>
-      <c r="G34" t="s">
+      <c r="H34" t="s">
         <v>149</v>
       </c>
-      <c r="H34" t="s">
+      <c r="I34" t="s">
         <v>150</v>
       </c>
     </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>4</v>
       </c>
@@ -2527,22 +2566,22 @@
         <v>0.56152267899999997</v>
       </c>
       <c r="D35" t="s">
-        <v>201</v>
-      </c>
-      <c r="E35" t="s">
+        <v>208</v>
+      </c>
+      <c r="F35" t="s">
         <v>151</v>
       </c>
-      <c r="F35" t="s">
+      <c r="G35" t="s">
         <v>152</v>
       </c>
-      <c r="G35" t="s">
+      <c r="H35" t="s">
         <v>153</v>
       </c>
-      <c r="H35" t="s">
+      <c r="I35" t="s">
         <v>154</v>
       </c>
     </row>
-    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>4</v>
       </c>
@@ -2550,22 +2589,22 @@
         <v>0.56194502000000002</v>
       </c>
       <c r="D36" t="s">
-        <v>201</v>
-      </c>
-      <c r="E36" t="s">
+        <v>208</v>
+      </c>
+      <c r="F36" t="s">
         <v>86</v>
       </c>
-      <c r="F36" t="s">
+      <c r="G36" t="s">
         <v>155</v>
       </c>
-      <c r="G36" t="s">
+      <c r="H36" t="s">
         <v>156</v>
       </c>
-      <c r="H36" t="s">
+      <c r="I36" t="s">
         <v>157</v>
       </c>
     </row>
-    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>4</v>
       </c>
@@ -2573,22 +2612,22 @@
         <v>0.56194502000000002</v>
       </c>
       <c r="D37" t="s">
-        <v>201</v>
-      </c>
-      <c r="E37" t="s">
+        <v>208</v>
+      </c>
+      <c r="F37" t="s">
         <v>158</v>
       </c>
-      <c r="F37" t="s">
+      <c r="G37" t="s">
         <v>159</v>
       </c>
-      <c r="G37" t="s">
+      <c r="H37" t="s">
         <v>160</v>
       </c>
-      <c r="H37" t="s">
+      <c r="I37" t="s">
         <v>161</v>
       </c>
     </row>
-    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>4</v>
       </c>
@@ -2596,22 +2635,22 @@
         <v>0.56194502000000002</v>
       </c>
       <c r="D38" t="s">
-        <v>201</v>
-      </c>
-      <c r="E38" t="s">
+        <v>208</v>
+      </c>
+      <c r="F38" t="s">
         <v>162</v>
       </c>
-      <c r="F38" t="s">
+      <c r="G38" t="s">
         <v>163</v>
       </c>
-      <c r="G38" t="s">
+      <c r="H38" t="s">
         <v>164</v>
       </c>
-      <c r="H38" t="s">
+      <c r="I38" t="s">
         <v>165</v>
       </c>
     </row>
-    <row r="39" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>4</v>
       </c>
@@ -2619,22 +2658,22 @@
         <v>0.56194502000000002</v>
       </c>
       <c r="D39" t="s">
-        <v>201</v>
-      </c>
-      <c r="E39" t="s">
+        <v>208</v>
+      </c>
+      <c r="F39" t="s">
         <v>166</v>
       </c>
-      <c r="F39" t="s">
+      <c r="G39" t="s">
         <v>167</v>
       </c>
-      <c r="G39" t="s">
+      <c r="H39" t="s">
         <v>168</v>
       </c>
-      <c r="H39" t="s">
+      <c r="I39" t="s">
         <v>157</v>
       </c>
     </row>
-    <row r="40" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>4</v>
       </c>
@@ -2642,25 +2681,28 @@
         <v>0.56194502000000002</v>
       </c>
       <c r="C40" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="D40" s="1">
         <v>1.0800000000000001E-2</v>
       </c>
-      <c r="E40" t="s">
+      <c r="E40" s="1" t="s">
+        <v>213</v>
+      </c>
+      <c r="F40" t="s">
         <v>169</v>
       </c>
-      <c r="F40" t="s">
+      <c r="G40" t="s">
         <v>170</v>
       </c>
-      <c r="G40" t="s">
+      <c r="H40" t="s">
         <v>171</v>
       </c>
-      <c r="H40" t="s">
+      <c r="I40" t="s">
         <v>172</v>
       </c>
     </row>
-    <row r="41" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>4</v>
       </c>
@@ -2668,22 +2710,22 @@
         <v>0.56194502000000002</v>
       </c>
       <c r="D41" t="s">
-        <v>201</v>
-      </c>
-      <c r="E41" t="s">
+        <v>208</v>
+      </c>
+      <c r="F41" t="s">
         <v>173</v>
       </c>
-      <c r="F41" t="s">
+      <c r="G41" t="s">
         <v>100</v>
       </c>
-      <c r="G41" t="s">
+      <c r="H41" t="s">
         <v>174</v>
       </c>
-      <c r="H41" t="s">
+      <c r="I41" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="42" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>4</v>
       </c>
@@ -2691,22 +2733,22 @@
         <v>0.56194502000000002</v>
       </c>
       <c r="D42" t="s">
-        <v>201</v>
-      </c>
-      <c r="E42" t="s">
+        <v>208</v>
+      </c>
+      <c r="F42" t="s">
         <v>175</v>
       </c>
-      <c r="F42" t="s">
+      <c r="G42" t="s">
         <v>176</v>
       </c>
-      <c r="G42" t="s">
+      <c r="H42" t="s">
         <v>177</v>
       </c>
-      <c r="H42" t="s">
+      <c r="I42" t="s">
         <v>178</v>
       </c>
     </row>
-    <row r="43" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A43">
         <v>5</v>
       </c>
@@ -2714,25 +2756,25 @@
         <v>0.74104780199999998</v>
       </c>
       <c r="D43" t="s">
-        <v>201</v>
-      </c>
-      <c r="E43" t="s">
+        <v>208</v>
+      </c>
+      <c r="F43" t="s">
         <v>179</v>
       </c>
-      <c r="F43" t="s">
+      <c r="G43" t="s">
         <v>180</v>
       </c>
-      <c r="G43" t="s">
+      <c r="H43" t="s">
         <v>181</v>
       </c>
-      <c r="H43" t="s">
+      <c r="I43" t="s">
         <v>182</v>
       </c>
-      <c r="I43" t="s">
+      <c r="J43" t="s">
         <v>183</v>
       </c>
     </row>
-    <row r="44" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A44">
         <v>5</v>
       </c>
@@ -2740,25 +2782,25 @@
         <v>0.74240941500000002</v>
       </c>
       <c r="D44" t="s">
-        <v>201</v>
-      </c>
-      <c r="E44" t="s">
+        <v>208</v>
+      </c>
+      <c r="F44" t="s">
         <v>131</v>
       </c>
-      <c r="F44" t="s">
+      <c r="G44" t="s">
         <v>184</v>
       </c>
-      <c r="G44" t="s">
+      <c r="H44" t="s">
         <v>185</v>
       </c>
-      <c r="H44" t="s">
+      <c r="I44" t="s">
         <v>186</v>
       </c>
-      <c r="I44" t="s">
+      <c r="J44" t="s">
         <v>187</v>
       </c>
     </row>
-    <row r="45" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A45">
         <v>4</v>
       </c>
@@ -2766,25 +2808,28 @@
         <v>0.79767161900000005</v>
       </c>
       <c r="C45" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="D45" s="1">
         <v>9.0300000000000005E-2</v>
       </c>
-      <c r="E45" t="s">
+      <c r="E45" s="1" t="s">
+        <v>214</v>
+      </c>
+      <c r="F45" t="s">
         <v>161</v>
       </c>
-      <c r="F45" t="s">
+      <c r="G45" t="s">
         <v>188</v>
       </c>
-      <c r="G45" t="s">
+      <c r="H45" t="s">
         <v>189</v>
       </c>
-      <c r="H45" t="s">
+      <c r="I45" t="s">
         <v>190</v>
       </c>
     </row>
-    <row r="46" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A46">
         <v>5</v>
       </c>
@@ -2792,24 +2837,27 @@
         <v>0.835514113</v>
       </c>
       <c r="C46" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="D46" s="1">
         <v>2.01E-2</v>
       </c>
-      <c r="E46" t="s">
+      <c r="E46" s="1" t="s">
+        <v>215</v>
+      </c>
+      <c r="F46" t="s">
         <v>191</v>
       </c>
-      <c r="F46" t="s">
+      <c r="G46" t="s">
         <v>192</v>
       </c>
-      <c r="G46" t="s">
+      <c r="H46" t="s">
         <v>193</v>
       </c>
-      <c r="H46" t="s">
+      <c r="I46" t="s">
         <v>194</v>
       </c>
-      <c r="I46" t="s">
+      <c r="J46" t="s">
         <v>195</v>
       </c>
     </row>

</xml_diff>